<commit_message>
se modifico la celda con un posible
</commit_message>
<xml_diff>
--- a/DATOS_VENTAS.xlsx
+++ b/DATOS_VENTAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TAREA_CERTUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFE1E9C-88CD-4A99-89DE-CA2F86BA4BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43359F27-1120-4E52-886B-54C5F033F2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE857284-433D-4F5E-8BA5-E1FF96EC809D}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>Fecha</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Puno</t>
-  </si>
-  <si>
-    <t>gato</t>
   </si>
 </sst>
 </file>
@@ -535,15 +532,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E083E8-5819-4521-8857-E05521BABE5D}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K9" sqref="K9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44928</v>
       </c>
@@ -578,7 +575,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44928</v>
       </c>
@@ -596,7 +593,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44928</v>
       </c>
@@ -613,11 +610,8 @@
       <c r="E4" s="5">
         <v>225</v>
       </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44928</v>
       </c>
@@ -635,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44928</v>
       </c>
@@ -653,7 +647,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44928</v>
       </c>
@@ -671,7 +665,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44929</v>
       </c>
@@ -689,7 +683,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44929</v>
       </c>
@@ -707,7 +701,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44929</v>
       </c>
@@ -725,7 +719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44929</v>
       </c>
@@ -743,7 +737,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44929</v>
       </c>
@@ -761,7 +755,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44930</v>
       </c>
@@ -779,7 +773,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44930</v>
       </c>
@@ -797,7 +791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44931</v>
       </c>

</xml_diff>